<commit_message>
Add: export search feature. Modify: update export for warehouse type
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -479,11 +479,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Product A</t>
+          <t>initial</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -495,7 +495,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Zone A</t>
+          <t>initial</t>
         </is>
       </c>
     </row>

</xml_diff>